<commit_message>
Add tab 28 report
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_28_rpt_PA_MultiYrStats.xlsx
+++ b/backend/reports/xlsx/Tab_28_rpt_PA_MultiYrStats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyleshapka/Development/github/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21F2D95-0CAF-9C4E-86F6-F58748A44EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B656413A-C8C8-0B44-8EB3-25F961263473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19700" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>{#r=d.report[i]}</t>
   </si>
@@ -50,16 +50,91 @@
     <t>{#date=d.date}</t>
   </si>
   <si>
-    <t>Project #</t>
-  </si>
-  <si>
-    <t>Project Name</t>
-  </si>
-  <si>
     <t>{#fy=d.fiscal_year}</t>
   </si>
   <si>
-    <t>Project ________ for {$fy} as of {$date}</t>
+    <t>Fiscal</t>
+  </si>
+  <si>
+    <t># of Projects</t>
+  </si>
+  <si>
+    <t>Total Budget</t>
+  </si>
+  <si>
+    <t>Total Recovered</t>
+  </si>
+  <si>
+    <t>Avg Duration</t>
+  </si>
+  <si>
+    <t># of CRs</t>
+  </si>
+  <si>
+    <t># w/ CRs</t>
+  </si>
+  <si>
+    <t>Avg. CR/Proj</t>
+  </si>
+  <si>
+    <t>Internal</t>
+  </si>
+  <si>
+    <t>External</t>
+  </si>
+  <si>
+    <t>Social Media</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Unique Clients</t>
+  </si>
+  <si>
+    <t>{$r.fiscal}</t>
+  </si>
+  <si>
+    <t>{$r1}</t>
+  </si>
+  <si>
+    <t>{$r.project_count}</t>
+  </si>
+  <si>
+    <t>{$r.total_project_budget}</t>
+  </si>
+  <si>
+    <t>{$r.total_recovered}</t>
+  </si>
+  <si>
+    <t>{$r.average_duration}</t>
+  </si>
+  <si>
+    <t>{$r.change_request_count}</t>
+  </si>
+  <si>
+    <t>{$r.average_cr_per_project}</t>
+  </si>
+  <si>
+    <t>{$r.internal_projects}</t>
+  </si>
+  <si>
+    <t>{$r.external_projects}</t>
+  </si>
+  <si>
+    <t>{$r.social_media_projects}</t>
+  </si>
+  <si>
+    <t>{$r.service_projects}</t>
+  </si>
+  <si>
+    <t>{$r.unique_client_count}</t>
+  </si>
+  <si>
+    <t>{d.portfolio_name} Multi-Year Project Statistics as of {$date}</t>
+  </si>
+  <si>
+    <t>{$r.projects_with_crs}</t>
   </si>
 </sst>
 </file>
@@ -69,7 +144,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -88,11 +163,6 @@
     </font>
     <font>
       <sz val="8.5"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
       <name val="BCSans-Regular"/>
     </font>
     <font>
@@ -201,17 +271,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -229,22 +293,17 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,10 +682,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B12"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -634,101 +693,145 @@
     <col min="1" max="1" width="11.1640625" customWidth="1"/>
     <col min="2" max="2" width="43.1640625" customWidth="1"/>
     <col min="3" max="9" width="15.83203125" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15" t="s">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="20" thickBot="1">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A2" s="6" t="s">
+      <c r="D2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="19">
+      <c r="B5" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="19">
+      <c r="B6" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="19">
+      <c r="B7" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="19">
+      <c r="B8" s="10"/>
+    </row>
+    <row r="9" spans="1:13" ht="19">
+      <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A3" s="4"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="9"/>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="9"/>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="7" spans="1:9" ht="19">
-      <c r="B7" s="16" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="19">
-      <c r="B8" s="16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="19">
-      <c r="B9" s="16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="19">
-      <c r="B10" s="16"/>
-    </row>
-    <row r="11" spans="1:9" ht="19">
-      <c r="B11" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="19">
-      <c r="B12" s="16" t="s">
+    </row>
+    <row r="10" spans="1:13" ht="19">
+      <c r="B10" s="10" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="C1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>